<commit_message>
Doi BH Hay Hue
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang1/5.DoiBH/DM230104_HayHue.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang1/5.DoiBH/DM230104_HayHue.xlsx
@@ -122,9 +122,6 @@
     <t>Người đại diện: Đại lý Hay Huế</t>
   </si>
   <si>
-    <t>TG102E</t>
-  </si>
-  <si>
     <t>Thiết bị thường xuyên mất tín hiệu</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Hà Nội, ngày 04 tháng 01 Năm 2023</t>
+  </si>
+  <si>
+    <t>TG102E1</t>
   </si>
 </sst>
 </file>
@@ -509,12 +509,90 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -523,84 +601,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -962,7 +962,7 @@
   <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="85" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -982,104 +982,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="18" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37"/>
-      <c r="B1" s="38"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="37" t="s">
+      <c r="A1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="39"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="40" t="s">
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
     </row>
     <row r="3" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="40" t="s">
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="45"/>
     </row>
     <row r="4" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="43" t="s">
+      <c r="A4" s="56"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="45"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="52"/>
     </row>
     <row r="6" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
     </row>
     <row r="8" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
@@ -1089,13 +1089,13 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
@@ -1105,15 +1105,15 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
     </row>
     <row r="11" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
@@ -1149,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12" s="30">
         <v>860906041230050</v>
@@ -1159,14 +1159,14 @@
         <v>22</v>
       </c>
       <c r="F12" s="31"/>
-      <c r="G12" s="61" t="s">
-        <v>33</v>
+      <c r="G12" s="32" t="s">
+        <v>32</v>
       </c>
       <c r="H12" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="62" t="s">
-        <v>34</v>
+      <c r="I12" s="33" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1186,49 +1186,49 @@
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
-      <c r="G14" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
+      <c r="G14" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
     </row>
     <row r="15" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="57" t="s">
+      <c r="H15" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="57"/>
+      <c r="I15" s="35"/>
     </row>
     <row r="16" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="60" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
       <c r="G16" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="60" t="s">
+      <c r="H16" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="60"/>
+      <c r="I16" s="38"/>
     </row>
     <row r="17" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
@@ -1268,35 +1268,47 @@
       <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58" t="s">
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
       <c r="G21" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="58" t="s">
+      <c r="H21" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="58"/>
+      <c r="I21" s="36"/>
       <c r="J21" s="15"/>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
     </row>
     <row r="22" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
     </row>
     <row r="63" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A1:C4"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="H21:I21"/>
@@ -1307,21 +1319,9 @@
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A1:C4"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:I10"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="1.5" bottom="1" header="0.43307086614173201" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="27" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="94" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>